<commit_message>
+Worked on downloaded path
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_2_A\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_2_f\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71432A41-6C51-49F3-9B7B-5864AC2C910D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7AFE1E-25CE-4FF2-9657-4FD3CDCD0945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -209,18 +209,6 @@
     <t>MonthlyReport</t>
   </si>
   <si>
-    <t>"Data\Input\"+MonthFolder.FullName</t>
-  </si>
-  <si>
-    <t>MonthlyReportsFolder</t>
-  </si>
-  <si>
-    <t>MonthlyReportPath</t>
-  </si>
-  <si>
-    <t>"Data\\Input\\MonthlyReport-"</t>
-  </si>
-  <si>
     <t>DownloadMonthlyReportNotLoading</t>
   </si>
   <si>
@@ -230,9 +218,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>MonthlyReportDownloadedPath</t>
-  </si>
-  <si>
     <t>PopNotAvailable</t>
   </si>
   <si>
@@ -251,12 +236,6 @@
     <t>YearlyReportUploadUrl</t>
   </si>
   <si>
-    <t>"C:\Users\hp\Documents\UiPath\Shireen_Capstone_2_Final\Data\Input\"+MonthFolder.FullName+"\"+month</t>
-  </si>
-  <si>
-    <t>"C:\Users\hp\Documents\UiPath\Shireen_Capstone_2_Final\Data\Output\Yearly-Report-2023-"+VendorId+".xlsx"</t>
-  </si>
-  <si>
     <t>AcmeCredentials</t>
   </si>
   <si>
@@ -300,6 +279,24 @@
   </si>
   <si>
     <t>Url for the ACME yearly report upload page</t>
+  </si>
+  <si>
+    <t>MonthlyReportDownloadPath</t>
+  </si>
+  <si>
+    <t>YearlyReportPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_2_f\Data\Output\Yearly-Report-2023-</t>
+  </si>
+  <si>
+    <t>C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_2_f\Data\Input\</t>
+  </si>
+  <si>
+    <t>Path where monthly downloaded report is present</t>
+  </si>
+  <si>
+    <t>Path where yearly report is present</t>
   </si>
 </sst>
 </file>
@@ -684,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -766,13 +763,13 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1776,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z986"/>
+  <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1968,7 +1965,7 @@
         <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
@@ -1979,7 +1976,7 @@
         <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
@@ -1990,7 +1987,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2001,7 +1998,7 @@
         <v>59</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -2012,7 +2009,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2023,7 +2020,7 @@
         <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
@@ -2034,7 +2031,7 @@
         <v>56</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
@@ -2045,110 +2042,102 @@
         <v>58</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="B26" t="s">
-        <v>61</v>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
         <v>63</v>
       </c>
-      <c r="B27" t="s">
-        <v>64</v>
+      <c r="B27">
+        <v>2023</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
         <v>65</v>
       </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
         <v>67</v>
       </c>
-      <c r="B29">
-        <v>2023</v>
+      <c r="B29" t="s">
+        <v>66</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
-        <v>75</v>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3083,10 +3072,6 @@
     <row r="980" ht="14.25" customHeight="1"/>
     <row r="981" ht="14.25" customHeight="1"/>
     <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>